<commit_message>
Variable has been more generalized. Now instead of just crack geometry, material properties can also be a variable
</commit_message>
<xml_diff>
--- a/Depth Damaged States Attenuation Model - Orientation =  30, Width = 2, Circumference = Outside, Axial Location = 235/PCs at A'.xlsx
+++ b/Depth Damaged States Attenuation Model - Orientation =  30, Width = 2, Circumference = Outside, Axial Location = 235/PCs at A'.xlsx
@@ -396,10 +396,10 @@
         <v>7000</v>
       </c>
       <c r="B2">
-        <v>0.01490264090467821</v>
+        <v>0.1681445254291393</v>
       </c>
       <c r="C2">
-        <v>0.1591395843146433</v>
+        <v>0.04385043669510873</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -407,10 +407,10 @@
         <v>7333.333333333333</v>
       </c>
       <c r="B3">
-        <v>-0.2986563237533446</v>
+        <v>0.3452536934207687</v>
       </c>
       <c r="C3">
-        <v>0.151676849945324</v>
+        <v>-0.1566425969469884</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -418,10 +418,10 @@
         <v>7666.666666666667</v>
       </c>
       <c r="B4">
-        <v>-0.2906122396347737</v>
+        <v>0.3556355745522564</v>
       </c>
       <c r="C4">
-        <v>-0.02824173524077874</v>
+        <v>0.1990384573524147</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -429,10 +429,10 @@
         <v>8000</v>
       </c>
       <c r="B5">
-        <v>-0.3281145509479111</v>
+        <v>0.431523411195365</v>
       </c>
       <c r="C5">
-        <v>0.211501873843282</v>
+        <v>-0.3941062953087233</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -440,10 +440,10 @@
         <v>8333.333333333334</v>
       </c>
       <c r="B6">
-        <v>-0.3039716987261208</v>
+        <v>0.360484414827775</v>
       </c>
       <c r="C6">
-        <v>0.2811253749722022</v>
+        <v>-0.02804511262863444</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -451,10 +451,10 @@
         <v>8666.666666666666</v>
       </c>
       <c r="B7">
-        <v>-0.2296047018793141</v>
+        <v>0.3972390355134647</v>
       </c>
       <c r="C7">
-        <v>0.110828291156707</v>
+        <v>-0.007063301683255129</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -462,10 +462,10 @@
         <v>9000</v>
       </c>
       <c r="B8">
-        <v>-0.4182722033376097</v>
+        <v>0.2321230097122929</v>
       </c>
       <c r="C8">
-        <v>0.2202326672929788</v>
+        <v>0.5083813793829081</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -473,10 +473,10 @@
         <v>9333.333333333334</v>
       </c>
       <c r="B9">
-        <v>-0.3547331146354348</v>
+        <v>0.1872709057121062</v>
       </c>
       <c r="C9">
-        <v>-0.02265700017467541</v>
+        <v>0.3528597334377797</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -484,10 +484,10 @@
         <v>9666.666666666666</v>
       </c>
       <c r="B10">
-        <v>-0.3330923015630856</v>
+        <v>0.2154501347641879</v>
       </c>
       <c r="C10">
-        <v>-0.2502208101602899</v>
+        <v>-0.4616186901550188</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -495,10 +495,10 @@
         <v>10000</v>
       </c>
       <c r="B11">
-        <v>-0.2319671901875477</v>
+        <v>0.1398838869808469</v>
       </c>
       <c r="C11">
-        <v>-0.462320714457904</v>
+        <v>0.2414382423752041</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -506,10 +506,10 @@
         <v>10333.33333333333</v>
       </c>
       <c r="B12">
-        <v>-0.2638721251665968</v>
+        <v>-0.04096520384890977</v>
       </c>
       <c r="C12">
-        <v>-0.3774735579209613</v>
+        <v>-0.1502088144699407</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -517,10 +517,10 @@
         <v>10666.66666666667</v>
       </c>
       <c r="B13">
-        <v>-0.1589197591813258</v>
+        <v>0.1113490370755945</v>
       </c>
       <c r="C13">
-        <v>-0.2716517930464554</v>
+        <v>-0.1770168458584153</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -528,10 +528,10 @@
         <v>11000</v>
       </c>
       <c r="B14">
-        <v>-0.0421477134382698</v>
+        <v>-0.04382704684561507</v>
       </c>
       <c r="C14">
-        <v>-0.2251291713706808</v>
+        <v>-0.1946009543459019</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -539,10 +539,10 @@
         <v>11333.33333333333</v>
       </c>
       <c r="B15">
-        <v>-0.02180512722634609</v>
+        <v>0.1445655189723084</v>
       </c>
       <c r="C15">
-        <v>-0.1188435388218479</v>
+        <v>0.01494890086795084</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -550,10 +550,10 @@
         <v>11666.66666666667</v>
       </c>
       <c r="B16">
-        <v>-0.06398371748483822</v>
+        <v>0.2439679294167482</v>
       </c>
       <c r="C16">
-        <v>0.3437201147738799</v>
+        <v>0.1772231259449329</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -561,10 +561,10 @@
         <v>12000</v>
       </c>
       <c r="B17">
-        <v>-0.08108200382717883</v>
+        <v>-0.02711960050508749</v>
       </c>
       <c r="C17">
-        <v>0.3003757736592653</v>
+        <v>-0.004815648980808656</v>
       </c>
     </row>
   </sheetData>

</xml_diff>